<commit_message>
add validation if payment ids duplicates in the file
</commit_message>
<xml_diff>
--- a/tests/unit/apps/payment/test_file/import_file_with_existing_delivery_date.xlsx
+++ b/tests/unit/apps/payment/test_file/import_file_with_existing_delivery_date.xlsx
@@ -94,7 +94,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -154,100 +154,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -272,31 +185,7 @@
     <xf numFmtId="59" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -568,7 +457,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -598,7 +486,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -624,7 +511,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -650,7 +536,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -676,7 +561,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -702,7 +586,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -728,7 +611,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -754,7 +636,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -780,7 +661,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -806,7 +686,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -863,7 +742,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -889,7 +767,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -915,7 +792,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -941,7 +817,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -967,7 +842,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -993,7 +867,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1019,7 +892,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1045,7 +917,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1071,7 +942,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1097,7 +967,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1145,7 +1014,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1175,7 +1043,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1201,7 +1068,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1227,7 +1093,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1253,7 +1118,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1279,7 +1143,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1305,7 +1168,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1331,7 +1193,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1357,7 +1218,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1383,7 +1243,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1409,7 +1268,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1525,82 +1384,27 @@
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="13"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="13"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="13"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
+      <c r="A5" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4">
+        <v>212</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1.84</v>
+      </c>
+      <c r="J5" s="4">
+        <v>150</v>
+      </c>
+      <c r="K5" s="8">
+        <v>45222</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>